<commit_message>
[ FIX SIGNED TYPE CONVERT ERROR , LEN = 32 + SIGNED NOT 100% = IEEE FLOAT ]
</commit_message>
<xml_diff>
--- a/CAN/CycleAndResponse.xlsx
+++ b/CAN/CycleAndResponse.xlsx
@@ -10,14 +10,14 @@
     <sheet name="K-Matrix " sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'K-Matrix '!$A$1:$AP$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'K-Matrix '!$A$1:$AP$8</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="61">
   <si>
     <t>Result</t>
   </si>
@@ -156,6 +156,39 @@
     <t>/</t>
   </si>
   <si>
+    <t>Vector__XXX</t>
+  </si>
+  <si>
+    <t>MinResponseTime</t>
+  </si>
+  <si>
+    <t>Analyze</t>
+  </si>
+  <si>
+    <t>0xDEAD1</t>
+  </si>
+  <si>
+    <t>intel</t>
+  </si>
+  <si>
+    <t>Signed</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>MaxResponseTime</t>
+  </si>
+  <si>
+    <t>CurResponseTime</t>
+  </si>
+  <si>
+    <t>AvgResponseTime</t>
+  </si>
+  <si>
     <t>SendCount</t>
   </si>
   <si>
@@ -165,19 +198,7 @@
     <t>0x100</t>
   </si>
   <si>
-    <t>intel</t>
-  </si>
-  <si>
-    <t>Unsigned</t>
-  </si>
-  <si>
     <t>X</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Vector__XXX</t>
   </si>
   <si>
     <t>ResponseCount</t>
@@ -244,13 +265,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -546,7 +570,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AP3"/>
+  <dimension ref="A1:AP7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -698,13 +722,13 @@
         <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>42</v>
@@ -716,10 +740,10 @@
         <v>42</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>42</v>
@@ -743,22 +767,22 @@
         <v>42</v>
       </c>
       <c r="R2" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="S2" s="2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T2" s="2">
         <v>33</v>
       </c>
       <c r="U2" s="2">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>42</v>
@@ -773,7 +797,7 @@
         <v>42</v>
       </c>
       <c r="AB2" s="2">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="AC2" s="2" t="s">
         <v>42</v>
@@ -788,12 +812,14 @@
         <v>0</v>
       </c>
       <c r="AG2" s="2">
-        <v>0</v>
+        <v>-327.68</v>
       </c>
       <c r="AH2" s="2">
-        <v>4294967295</v>
-      </c>
-      <c r="AI2" s="2"/>
+        <v>327.67</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2" t="s">
         <v>42</v>
@@ -806,136 +832,630 @@
       </c>
       <c r="AN2" s="2"/>
       <c r="AO2" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AP2" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:42">
-      <c r="A3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="A3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O3" s="3">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R3" s="3">
+        <v>8</v>
+      </c>
+      <c r="S3" s="3">
+        <v>32</v>
+      </c>
+      <c r="T3" s="3">
+        <v>49</v>
+      </c>
+      <c r="U3" s="3">
+        <v>16</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="3">
+        <v>-327.68</v>
+      </c>
+      <c r="AH3" s="3">
+        <v>327.67</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ3" s="3"/>
+      <c r="AK3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN3" s="3"/>
+      <c r="AO3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP3" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42">
+      <c r="A4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R4" s="3">
+        <v>8</v>
+      </c>
+      <c r="S4" s="3">
+        <v>0</v>
+      </c>
+      <c r="T4" s="3">
+        <v>17</v>
+      </c>
+      <c r="U4" s="3">
+        <v>16</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="3">
+        <v>-327.68</v>
+      </c>
+      <c r="AH4" s="3">
+        <v>327.67</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ4" s="3"/>
+      <c r="AK4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN4" s="3"/>
+      <c r="AO4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP4" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42">
+      <c r="A5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R5" s="3">
+        <v>8</v>
+      </c>
+      <c r="S5" s="3">
+        <v>48</v>
+      </c>
+      <c r="T5" s="3">
+        <v>65</v>
+      </c>
+      <c r="U5" s="3">
+        <v>16</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="3">
+        <v>-327.68</v>
+      </c>
+      <c r="AH5" s="3">
+        <v>327.67</v>
+      </c>
+      <c r="AI5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ5" s="3"/>
+      <c r="AK5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN5" s="3"/>
+      <c r="AO5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP5" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42">
+      <c r="A6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R6" s="2">
+        <v>4</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0</v>
+      </c>
+      <c r="T6" s="2">
+        <v>33</v>
+      </c>
+      <c r="U6" s="2">
+        <v>32</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="2">
+        <v>-2147483648</v>
+      </c>
+      <c r="AH6" s="2">
+        <v>2147483647</v>
+      </c>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN6" s="2"/>
+      <c r="AO6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O3" s="2">
-        <v>0</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="R3" s="2">
+    </row>
+    <row r="7" spans="1:42">
+      <c r="A7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R7" s="2">
         <v>4</v>
       </c>
-      <c r="S3" s="2">
-        <v>0</v>
-      </c>
-      <c r="T3" s="2">
+      <c r="S7" s="2">
+        <v>0</v>
+      </c>
+      <c r="T7" s="2">
         <v>33</v>
       </c>
-      <c r="U3" s="2">
+      <c r="U7" s="2">
         <v>32</v>
       </c>
-      <c r="V3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="W3" s="2" t="s">
+      <c r="V7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="X3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB3" s="2">
+      <c r="W7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB7" s="2">
         <v>1</v>
       </c>
-      <c r="AC3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="2">
-        <v>4294967295</v>
-      </c>
-      <c r="AI3" s="2"/>
-      <c r="AJ3" s="2"/>
-      <c r="AK3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AM3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN3" s="2"/>
-      <c r="AO3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AP3" s="2" t="s">
-        <v>49</v>
+      <c r="AC7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="2">
+        <v>-2147483648</v>
+      </c>
+      <c r="AH7" s="2">
+        <v>2147483647</v>
+      </c>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN7" s="2"/>
+      <c r="AO7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP7" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AP4"/>
+  <autoFilter ref="A1:AP8"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>